<commit_message>
142 en 2 30
</commit_message>
<xml_diff>
--- a/pilotos.xlsx
+++ b/pilotos.xlsx
@@ -1555,7 +1555,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2713,7 +2713,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="3" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
166 va a 168
</commit_message>
<xml_diff>
--- a/pilotos.xlsx
+++ b/pilotos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Clasica" sheetId="1" state="visible" r:id="rId3"/>
@@ -1554,7 +1554,7 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -3272,8 +3272,8 @@
   </sheetPr>
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4030,7 +4030,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B38" s="3" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
108 SS en 2,20
</commit_message>
<xml_diff>
--- a/pilotos.xlsx
+++ b/pilotos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Clasica" sheetId="1" state="visible" r:id="rId3"/>
@@ -3272,7 +3272,7 @@
   </sheetPr>
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -4470,8 +4470,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4774,7 +4774,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>214</v>
+        <v>7</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>35</v>

</xml_diff>